<commit_message>
re sync with github
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/Location_Types.xlsx
+++ b/utils/config/ReferenceLists/Location_Types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/jeremy_krogh_gov_bc_ca/Documents/Projects/2025/github_projects/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{FA2B1C84-549E-4420-BDF2-E354C2540A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F89CDBC1-8FCB-4469-8B1B-94D4CA1FC5F0}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{FA2B1C84-549E-4420-BDF2-E354C2540A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29F0F568-DC6D-49CE-B54B-E9595AEE2424}"/>
   <bookViews>
-    <workbookView xWindow="-17420" yWindow="1780" windowWidth="14400" windowHeight="8260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14685" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Location_Types" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>customId</t>
   </si>
@@ -117,6 +117,87 @@
   </si>
   <si>
     <t>Septic Tank</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>A sampling location within a facility that is not better described by any other location type.</t>
+  </si>
+  <si>
+    <t>An anthropogenic body of water designed to disperse into the underlying soil, typically for pollution abatement.</t>
+  </si>
+  <si>
+    <t>A sewer system that carries a mixture of stormwater and sanitary sewage.</t>
+  </si>
+  <si>
+    <t>The ocean or open sea.</t>
+  </si>
+  <si>
+    <t>A land-based sampling location for soil, soil vapor, plants, etc.</t>
+  </si>
+  <si>
+    <t>A location where groundwater naturally emerges at the surface.</t>
+  </si>
+  <si>
+    <t>Any type of groundwater well.</t>
+  </si>
+  <si>
+    <t>A sewer system that carries stormwater only, not combined or sanitary sewage.</t>
+  </si>
+  <si>
+    <t>A brackish water zone where a river meets the ocean.</t>
+  </si>
+  <si>
+    <t>Water seeping from the ground, sometimes forming small pools.</t>
+  </si>
+  <si>
+    <t>A sewer system that carries only sanitary (wastewater) flow, not combined with stormwater.</t>
+  </si>
+  <si>
+    <t>A site containing samples of refuse or related sediments.</t>
+  </si>
+  <si>
+    <t>A naturally flowing body of fresh water.</t>
+  </si>
+  <si>
+    <t>A point where air emissions are sampled near or at their release into the atmosphere.</t>
+  </si>
+  <si>
+    <t>An anthropogenic trench or pipe used to drain stormwater.</t>
+  </si>
+  <si>
+    <t>Similar to a terrestrial location, but specifically used for agricultural purposes.</t>
+  </si>
+  <si>
+    <t>A location at or very near where wastewater is discharged into the environment.</t>
+  </si>
+  <si>
+    <t>An area with buried perforated pipes used to drain saturated soil.</t>
+  </si>
+  <si>
+    <t>A site established to monitor air quality and related parameters.</t>
+  </si>
+  <si>
+    <t>Water or solids applied to land for irrigation or disposal.</t>
+  </si>
+  <si>
+    <t>An anthropogenic pond designed to slow and temporarily hold runoff, typically for pollution control.</t>
+  </si>
+  <si>
+    <t>A sampling point near a storage facility, often for industrial or waste monitoring.</t>
+  </si>
+  <si>
+    <t>A well used to inject wastewater into an aquifer.</t>
+  </si>
+  <si>
+    <t>The burning of waste or vegetation (slash) in the open air.</t>
+  </si>
+  <si>
+    <t>A tank used to separate and collect solids from liquid household wastewater.</t>
+  </si>
+  <si>
+    <t>A natural or anthropogenic body of fresh water, not used for wastewater storage or disposal.</t>
   </si>
 </sst>
 </file>
@@ -469,148 +550,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.81640625" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="128.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>